<commit_message>
Agregamos nuggets, mapeamos toda la bd con scaffolding,  y creamos el metodo get de la tabla clientes en el controlador Cliente del WS API REST
</commit_message>
<xml_diff>
--- a/PasosExcel.xlsx
+++ b/PasosExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\source\repos\VentasReal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.ardilar\source\repos\VentasReal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AF36E2-C967-43FD-9164-B9483A6D546B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081C3CDD-7694-4440-B218-8B401527213C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0B3D9CDD-2541-476F-89B2-848D864A77F2}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{0B3D9CDD-2541-476F-89B2-848D864A77F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Sistema de ventas real C# .Net core, angular y xamarin, curso HdeLeon</t>
   </si>
@@ -50,6 +50,45 @@
   </si>
   <si>
     <t>draw.io</t>
+  </si>
+  <si>
+    <t>Comandos Consola</t>
+  </si>
+  <si>
+    <t>PROYECTO</t>
+  </si>
+  <si>
+    <t>DIAGRAMA</t>
+  </si>
+  <si>
+    <t>ARCHIVO SQL</t>
+  </si>
+  <si>
+    <t>BDSQLServer</t>
+  </si>
+  <si>
+    <t>SQL Server</t>
+  </si>
+  <si>
+    <t>nugets</t>
+  </si>
+  <si>
+    <t>Conexión BD con autentificacion de windows</t>
+  </si>
+  <si>
+    <t>Conexión BD sin autentificacion de windows</t>
+  </si>
+  <si>
+    <t>Scaffold-DBContext "Server=OFITE-GRUDE8\SQLEXPRESS;Database=VentaReal;Trusted_Connection=True;" Microsoft.EntityFrameworkCore.SqlServer -OutputDir Models</t>
+  </si>
+  <si>
+    <t>Scaffold-DBContext "Server=OFITE-GRUDE8\SQLEXPRESS;Database=VentaReal;Trusted_Connection=False;user=sa;Password=abc123;" Microsoft.EntityFrameworkCore.SqlServer -OutputDir Models</t>
+  </si>
+  <si>
+    <t>Microsoft.EntityFrameworkCore.SqlServer 3.1.21</t>
+  </si>
+  <si>
+    <t>Microsoft.EntityFrameworkCore.Tools 3.1.21</t>
   </si>
 </sst>
 </file>
@@ -65,7 +104,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +123,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -97,12 +142,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -419,15 +467,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1F61C6-6635-46CD-BBF1-A54A5BACF429}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -448,27 +500,77 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>3</v>
       </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Configuracion HttpGet -en el startup de WSVenta se configuro para que acepte el CORS -en el proyecto de angular genere un nuevo servicio para el protocolo HttpGet y asi obtener los datos de la api/Clientes, recordar que .net debe estar corriendo para que funcione esta solicictud
</commit_message>
<xml_diff>
--- a/PasosExcel.xlsx
+++ b/PasosExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.ardilar\source\repos\VentasReal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081C3CDD-7694-4440-B218-8B401527213C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0368258-35D4-482A-8525-4EDA0E54C8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{0B3D9CDD-2541-476F-89B2-848D864A77F2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Sistema de ventas real C# .Net core, angular y xamarin, curso HdeLeon</t>
   </si>
@@ -89,13 +89,63 @@
   </si>
   <si>
     <t>Microsoft.EntityFrameworkCore.Tools 3.1.21</t>
+  </si>
+  <si>
+    <t>Angular/Ventas/App</t>
+  </si>
+  <si>
+    <t>ng add @angular/material</t>
+  </si>
+  <si>
+    <t>instalar plantilla de angular</t>
+  </si>
+  <si>
+    <t>ng generate component Home</t>
+  </si>
+  <si>
+    <t>crear componente</t>
+  </si>
+  <si>
+    <t>ng generate module app-routing --flat --module=app</t>
+  </si>
+  <si>
+    <t>agregar enrutamiento al proyecto app</t>
+  </si>
+  <si>
+    <t>Configuración</t>
+  </si>
+  <si>
+    <t>Startup.cs</t>
+  </si>
+  <si>
+    <r>
+      <t>CORS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF202124"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (Cross Origin Resource Sharing, o bien en español Intercambio de Recursos de Origen Cruzado)</t>
+    </r>
+  </si>
+  <si>
+    <t>services.AddCors(opciones =&gt;</t>
+  </si>
+  <si>
+    <t>ng generate service services/apiCliente</t>
+  </si>
+  <si>
+    <t>crear un servicio; si hay error colocar al inicio npm run</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,8 +153,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +192,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -142,8 +211,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -153,6 +223,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1F61C6-6635-46CD-BBF1-A54A5BACF429}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,30 +555,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -519,14 +593,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -546,6 +620,15 @@
       <c r="E5" t="s">
         <v>13</v>
       </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -566,12 +649,52 @@
         <v>18</v>
       </c>
     </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se configuro el JWT en .net core API, donde se crearon nuevas clases e interfaces.
</commit_message>
<xml_diff>
--- a/PasosExcel.xlsx
+++ b/PasosExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.ardilar\source\repos\VentasReal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\source\repos\VentasReal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0368258-35D4-482A-8525-4EDA0E54C8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA09049-A5BB-448F-BD4D-4C1B38E9E3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{0B3D9CDD-2541-476F-89B2-848D864A77F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0B3D9CDD-2541-476F-89B2-848D864A77F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Sistema de ventas real C# .Net core, angular y xamarin, curso HdeLeon</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>crear un servicio; si hay error colocar al inicio npm run</t>
+  </si>
+  <si>
+    <t>Agregar tablas al modelo: "table1", "table2", "table3"</t>
+  </si>
+  <si>
+    <t>Scaffold-DBContext "Server=OFITE-GRUDE8\SQLEXPRESS;Database=VentaReal;Trusted_Connection=True;" Microsoft.EntityFrameworkCore.SqlServer -OutputDir Models -Tables "Usuario" -Force</t>
+  </si>
+  <si>
+    <t>Microsoft.AspNetCore.Authentication.JwtBearer 3.0.3</t>
+  </si>
+  <si>
+    <t>System.IdentityModel.Tokens.Jwt 6.6.0</t>
   </si>
 </sst>
 </file>
@@ -167,7 +179,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +210,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -211,9 +229,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -223,8 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1F61C6-6635-46CD-BBF1-A54A5BACF429}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,32 +574,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -626,15 +645,15 @@
       <c r="G5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
@@ -645,45 +664,61 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E13" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se implemento el componente login en angular
</commit_message>
<xml_diff>
--- a/PasosExcel.xlsx
+++ b/PasosExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\source\repos\VentasReal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.ardilar\source\repos\VentasReal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA09049-A5BB-448F-BD4D-4C1B38E9E3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE0729F-8A8E-4A72-A9DD-9FE7AD1BE243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0B3D9CDD-2541-476F-89B2-848D864A77F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B3D9CDD-2541-476F-89B2-848D864A77F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Sistema de ventas real C# .Net core, angular y xamarin, curso HdeLeon</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>System.IdentityModel.Tokens.Jwt 6.6.0</t>
+  </si>
+  <si>
+    <t>OFITE-GRUDE8\\SQLEXPRESS</t>
+  </si>
+  <si>
+    <t>localhost</t>
   </si>
 </sst>
 </file>
@@ -234,6 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -243,7 +250,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1F61C6-6635-46CD-BBF1-A54A5BACF429}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,31 +580,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -650,10 +656,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
@@ -664,7 +670,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D7" t="s">
@@ -675,12 +681,12 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -720,6 +726,16 @@
       </c>
       <c r="E13" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#21 Maestro detalle en angular enviar información de la venta y los conceptos al backend, --como se envia esta información en string al backend, se implementaron dos clases en la carpeta tools y se configuran el startup para que todos los datos recibidos en string se conviertan en int o decimal segun sea el caso para recibirlos.
</commit_message>
<xml_diff>
--- a/PasosExcel.xlsx
+++ b/PasosExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.ardilar\source\repos\VentasReal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\source\repos\VentasReal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE0729F-8A8E-4A72-A9DD-9FE7AD1BE243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972FD1DF-0A7A-45A8-B668-84C473EC0AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B3D9CDD-2541-476F-89B2-848D864A77F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0B3D9CDD-2541-476F-89B2-848D864A77F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Sistema de ventas real C# .Net core, angular y xamarin, curso HdeLeon</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>instalar plantilla de angular</t>
-  </si>
-  <si>
-    <t>ng generate component Home</t>
   </si>
   <si>
     <t>crear componente</t>
@@ -157,6 +154,15 @@
   </si>
   <si>
     <t>localhost</t>
+  </si>
+  <si>
+    <t>npm install</t>
+  </si>
+  <si>
+    <t>recompilar despues de hacer pull en git</t>
+  </si>
+  <si>
+    <t>"npm run" ng generate component Home</t>
   </si>
 </sst>
 </file>
@@ -567,7 +573,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +608,7 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="2"/>
@@ -646,13 +652,13 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -674,20 +680,20 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -706,36 +712,44 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
         <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
         <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
         <v>30</v>
       </c>
-      <c r="E13" t="s">
-        <v>31</v>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>